<commit_message>
ENH:finish work of LexicalAnalyzer
</commit_message>
<xml_diff>
--- a/Docs/C-词法分析表.xlsx
+++ b/Docs/C-词法分析表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="101">
   <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -396,6 +396,22 @@
   </si>
   <si>
     <t>-15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-18</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -515,9 +531,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -525,6 +538,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -823,20 +839,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:CA26"/>
+    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:CB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="9"/>
-    <col min="2" max="53" width="9" style="10"/>
-    <col min="54" max="63" width="9" style="11"/>
-    <col min="64" max="79" width="9" style="12"/>
-    <col min="80" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="9" style="4"/>
+    <col min="2" max="53" width="9" style="9"/>
+    <col min="54" max="63" width="9" style="10"/>
+    <col min="64" max="79" width="9" style="11"/>
+    <col min="80" max="80" width="9" style="12"/>
+    <col min="81" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" s="2" customFormat="1">
+    <row r="1" spans="1:80" s="2" customFormat="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1072,8 +1089,11 @@
       <c r="CA1" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="CB1" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="2" spans="1:79">
+    <row r="2" spans="1:80">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1311,8 +1331,11 @@
       <c r="CA2" s="7">
         <v>25</v>
       </c>
+      <c r="CB2" s="12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:79">
+    <row r="3" spans="1:80">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1550,8 +1573,11 @@
       <c r="CA3" s="7">
         <v>-1</v>
       </c>
+      <c r="CB3" s="12">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="4" spans="1:79">
+    <row r="4" spans="1:80">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1789,8 +1815,11 @@
       <c r="CA4" s="7" t="s">
         <v>71</v>
       </c>
+      <c r="CB4" s="12">
+        <v>-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:79">
+    <row r="5" spans="1:80">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2028,8 +2057,11 @@
       <c r="CA5" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="CB5" s="12">
+        <v>-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:79">
+    <row r="6" spans="1:80">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2267,8 +2299,11 @@
       <c r="CA6" s="5" t="s">
         <v>72</v>
       </c>
+      <c r="CB6" s="12">
+        <v>-4</v>
+      </c>
     </row>
-    <row r="7" spans="1:79">
+    <row r="7" spans="1:80">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2506,8 +2541,11 @@
       <c r="CA7" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="CB7" s="12">
+        <v>-5</v>
+      </c>
     </row>
-    <row r="8" spans="1:79">
+    <row r="8" spans="1:80">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2745,8 +2783,11 @@
       <c r="CA8" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="CB8" s="12">
+        <v>-7</v>
+      </c>
     </row>
-    <row r="9" spans="1:79">
+    <row r="9" spans="1:80">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2984,8 +3025,11 @@
       <c r="CA9" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="CB9" s="12">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:79">
+    <row r="10" spans="1:80">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3223,8 +3267,11 @@
       <c r="CA10" s="5" t="s">
         <v>68</v>
       </c>
+      <c r="CB10" s="12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:79">
+    <row r="11" spans="1:80">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3462,8 +3509,11 @@
       <c r="CA11" s="5" t="s">
         <v>78</v>
       </c>
+      <c r="CB11" s="12">
+        <v>-9</v>
+      </c>
     </row>
-    <row r="12" spans="1:79">
+    <row r="12" spans="1:80">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3701,8 +3751,11 @@
       <c r="CA12" s="5" t="s">
         <v>80</v>
       </c>
+      <c r="CB12" s="12">
+        <v>-8</v>
+      </c>
     </row>
-    <row r="13" spans="1:79">
+    <row r="13" spans="1:80">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3940,8 +3993,11 @@
       <c r="CA13" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="CB13" s="12">
+        <v>-11</v>
+      </c>
     </row>
-    <row r="14" spans="1:79">
+    <row r="14" spans="1:80">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -4179,8 +4235,11 @@
       <c r="CA14" s="5" t="s">
         <v>90</v>
       </c>
+      <c r="CB14" s="12">
+        <v>-10</v>
+      </c>
     </row>
-    <row r="15" spans="1:79">
+    <row r="15" spans="1:80">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -4418,8 +4477,11 @@
       <c r="CA15" s="5" t="s">
         <v>91</v>
       </c>
+      <c r="CB15" s="12">
+        <v>-13</v>
+      </c>
     </row>
-    <row r="16" spans="1:79">
+    <row r="16" spans="1:80">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -4656,6 +4718,9 @@
       </c>
       <c r="CA16" s="5" t="s">
         <v>93</v>
+      </c>
+      <c r="CB16" s="12">
+        <v>-12</v>
       </c>
     </row>
     <row r="17" spans="1:82">
@@ -4896,6 +4961,9 @@
       <c r="CA17" s="5" t="s">
         <v>68</v>
       </c>
+      <c r="CB17" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:82">
       <c r="A18" s="4">
@@ -5135,6 +5203,9 @@
       <c r="CA18" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="CB18" s="12">
+        <v>-14</v>
+      </c>
     </row>
     <row r="19" spans="1:82">
       <c r="A19" s="4">
@@ -5374,6 +5445,9 @@
       <c r="CA19" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="CB19" s="12">
+        <v>-15</v>
+      </c>
     </row>
     <row r="20" spans="1:82">
       <c r="A20" s="4">
@@ -5613,7 +5687,9 @@
       <c r="CA20" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="CB20" s="5"/>
+      <c r="CB20" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="CC20" s="5"/>
       <c r="CD20" s="5"/>
     </row>
@@ -5855,7 +5931,9 @@
       <c r="CA21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="CB21" s="5"/>
+      <c r="CB21" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="CC21" s="5"/>
       <c r="CD21" s="5"/>
     </row>
@@ -6097,7 +6175,9 @@
       <c r="CA22" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="CB22" s="5"/>
+      <c r="CB22" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="CC22" s="5"/>
       <c r="CD22" s="5"/>
     </row>
@@ -6339,7 +6419,9 @@
       <c r="CA23" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="CB23" s="5"/>
+      <c r="CB23" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="CC23" s="5"/>
       <c r="CD23" s="5"/>
     </row>
@@ -6581,7 +6663,9 @@
       <c r="CA24" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="CB24" s="5"/>
+      <c r="CB24" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="CC24" s="5"/>
       <c r="CD24" s="5"/>
     </row>
@@ -6823,7 +6907,9 @@
       <c r="CA25" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="CB25" s="5"/>
+      <c r="CB25" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="CC25" s="5"/>
       <c r="CD25" s="5"/>
     </row>
@@ -7065,7 +7151,9 @@
       <c r="CA26" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="CB26" s="5"/>
+      <c r="CB26" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="CC26" s="5"/>
       <c r="CD26" s="5"/>
     </row>

</xml_diff>